<commit_message>
Suggest exiftool command ' exiftool -X -a -ext wav -struct -charset riff=utf8 "fileDirectory" > "output.xml" ' Less burdensome message generation Generate complete manifest from series + format or cavafy API Choose outputs (default all) Boilerplate values have llower preference Warn of potential duplicate assets Generate CSV of errors, including OK assets Parse CodingHistory Broader LoC subjects not automatically applied Add instantiationRelation 'Is Dub Of' Default collation: http://www.w3.org/2013/collation/UCA?ignore-symbols=yes;strength=primary Concatenate CMS segments info Catch non-Microsoft PCM codec Merge source instantiation into destination asset Generate Title Case
</commit_message>
<xml_diff>
--- a/currentTemplates/rdfMasterTemplate.xlsx
+++ b/currentTemplates/rdfMasterTemplate.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\02 CATALOGING\Instantiation uploads\nypr-archives-ingest-scripts\currentTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A94747A-B4BD-4324-8704-4B7DD6C41A4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44652658-E8F5-4486-A79B-533A8ACAECD7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" tabRatio="703" activeTab="3" xr2:uid="{D22D536D-03EF-4533-83EF-1BF9643EA422}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="703" activeTab="3" xr2:uid="{D22D536D-03EF-4533-83EF-1BF9643EA422}"/>
   </bookViews>
   <sheets>
-    <sheet name="masterRDF" sheetId="8" r:id="rId1"/>
-    <sheet name="01_Inventory" sheetId="12" r:id="rId2"/>
-    <sheet name="Example" sheetId="2" r:id="rId3"/>
-    <sheet name="02_FixMD" sheetId="13" r:id="rId4"/>
+    <sheet name="00_MasterData" sheetId="14" r:id="rId1"/>
+    <sheet name="Example" sheetId="2" r:id="rId2"/>
+    <sheet name="01_Inventory" sheetId="12" r:id="rId3"/>
+    <sheet name="02_FixMD" sheetId="8" r:id="rId4"/>
     <sheet name="instantiationIDs" sheetId="5" r:id="rId5"/>
     <sheet name="instructions" sheetId="7" r:id="rId6"/>
     <sheet name="vocabularies" sheetId="6" r:id="rId7"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="139">
   <si>
     <t>ns1:about</t>
   </si>
@@ -479,6 +479,30 @@
   </si>
   <si>
     <t>photoLocator</t>
+  </si>
+  <si>
+    <t>photoLocation</t>
+  </si>
+  <si>
+    <t>futureLocation</t>
+  </si>
+  <si>
+    <t>currentLocation</t>
+  </si>
+  <si>
+    <t>shipmentSendDate</t>
+  </si>
+  <si>
+    <t>shipmentReturnDate</t>
+  </si>
+  <si>
+    <t>binID</t>
+  </si>
+  <si>
+    <t>boxID</t>
+  </si>
+  <si>
+    <t>shipmentID</t>
   </si>
 </sst>
 </file>
@@ -538,7 +562,160 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="63">
+  <dxfs count="110">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -574,18 +751,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -953,176 +1118,226 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{152F4DBB-82EC-4174-B546-903AE163E78E}" name="Table9" displayName="Table9" ref="N1:BF2" tableType="xml" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61" connectionId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F5B8D297-B61D-44B7-97F3-B2353943E960}" name="Table92" displayName="Table92" ref="N1:BF2" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
   <autoFilter ref="N1:BF2" xr:uid="{DBA4640A-ED60-420F-906F-CF4D7DD1EE4D}"/>
   <tableColumns count="45">
-    <tableColumn id="1" xr3:uid="{A580D164-B803-461C-9F4F-A5883098A8DC}" uniqueName="ns1:about" name="ns1:about" dataDxfId="60">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/@ns1:about" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="2" xr3:uid="{05AC7C08-38B5-4261-A443-BEA6080FEDDA}" uniqueName="ns13:toolkit" name="ns13:toolkit" dataDxfId="59">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/@ns13:toolkit" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{A5EA5A7D-DF33-4A97-82BB-0A7F0753F4DF}" uniqueName="ns9:FileName" name="ns9:FileName" dataDxfId="58">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns9:FileName" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{EA4A8834-6D73-4C7F-B6AF-389D2D43DD68}" uniqueName="ns9:Directory" name="ns9:Directory" dataDxfId="57">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns9:Directory" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{67463FDA-5FD6-4B14-9F81-FE55D0178052}" uniqueName="ns9:FileSize" name="ns9:FileSize" dataDxfId="56">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns9:FileSize" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{0C3060F6-F8A0-4D82-AAC7-1BDA75963948}" uniqueName="ns9:FileModifyDate" name="ns9:FileModifyDate" dataDxfId="55">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns9:FileModifyDate" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{D8247E8D-6713-454E-918C-65CF07DFD18E}" uniqueName="ns9:FileAccessDate" name="ns9:FileAccessDate" dataDxfId="54">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns9:FileAccessDate" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{314C7B67-1EA1-4F9B-9BA8-65CEF7058C26}" uniqueName="ns9:FileCreateDate" name="ns9:FileCreateDate" dataDxfId="53">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns9:FileCreateDate" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{FE9CC9E5-2BD9-46CA-8DDF-367714039F6E}" uniqueName="ns9:FilePermissions" name="ns9:FilePermissions" dataDxfId="52">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns9:FilePermissions" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="10" xr3:uid="{A745FD77-9ADB-44D6-8904-007E5A609840}" uniqueName="ns10:FileType" name="ns10:FileType" dataDxfId="51">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns10:FileType" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="11" xr3:uid="{BC259896-1D6F-4AE7-A726-B8834A69BBC2}" uniqueName="ns10:FileTypeExtension" name="ns10:FileTypeExtension" dataDxfId="50">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns10:FileTypeExtension" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="12" xr3:uid="{BBE38AEA-ECEB-4766-8AB0-933A72D382A8}" uniqueName="ns10:MIMEType" name="ns10:MIMEType" dataDxfId="49">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns10:MIMEType" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="13" xr3:uid="{39257707-B95F-45C9-AC76-F1FCA3BBF450}" uniqueName="ns8:Description" name="ns8:Description" dataDxfId="48">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Description" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="14" xr3:uid="{9CA1E0C7-3686-4C63-B1BF-25AB0784699E}" uniqueName="ns8:Originator" name="ns8:Originator" dataDxfId="47">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Originator" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="15" xr3:uid="{7087961F-8AA4-489C-9EF6-98485712B62A}" uniqueName="ns8:OriginatorReference" name="ns8:OriginatorReference" dataDxfId="46">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:OriginatorReference" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="16" xr3:uid="{C73D8355-013C-400C-A0A9-EFE01E3D050B}" uniqueName="ns8:Artist" name="ns8:Artist" dataDxfId="45">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Artist" xmlDataType="anyURI"/>
-    </tableColumn>
-    <tableColumn id="17" xr3:uid="{D13DCDF0-0CC2-4BCB-AFDF-2CF798AFE524}" uniqueName="ns8:Commissioned" name="ns8:Commissioned" dataDxfId="44">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Commissioned" xmlDataType="anyURI"/>
-    </tableColumn>
-    <tableColumn id="18" xr3:uid="{02063AF9-BF3F-4FF1-8D86-A9A5A1240A73}" uniqueName="ns8:DateCreated" name="ns8:DateCreated" dataDxfId="43">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:DateCreated" xmlDataType="date"/>
-    </tableColumn>
-    <tableColumn id="19" xr3:uid="{BB997E4E-ED1D-4A6D-8A24-A863681A2E20}" uniqueName="ns8:Keywords" name="ns8:Keywords" dataDxfId="42">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Keywords" xmlDataType="anyURI"/>
-    </tableColumn>
-    <tableColumn id="20" xr3:uid="{48BC8FF1-7BFE-41C9-9C48-F8DC04E14800}" uniqueName="ns8:Subject" name="ns8:Subject" dataDxfId="41">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Subject" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="21" xr3:uid="{5120FA96-3590-4F48-8545-6E4CC51A5B49}" uniqueName="ns8:Software" name="ns8:Software" dataDxfId="40">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Software" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="22" xr3:uid="{58933FB6-0CDD-4BB3-837C-451A48F41091}" uniqueName="ns8:Source" name="ns8:Source" dataDxfId="39">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Source" xmlDataType="anyURI"/>
-    </tableColumn>
-    <tableColumn id="23" xr3:uid="{6DB07D3F-F109-424F-9423-952C9C1F0F68}" uniqueName="ns8:ArchivalLocation" name="ns8:ArchivalLocation" dataDxfId="38">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:ArchivalLocation" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="24" xr3:uid="{32999CD4-C6BA-4922-B7AA-328EC1D95C5C}" uniqueName="ns8:Comment" name="ns8:Comment" dataDxfId="37">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Comment" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="25" xr3:uid="{88B06FCA-C7DB-4AFE-8C8A-9156B064162B}" uniqueName="ns8:Copyright" name="ns8:Copyright" dataDxfId="36">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Copyright" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="26" xr3:uid="{78765629-CBE4-402A-9D4E-E90C72C8BF39}" uniqueName="ns8:Engineer" name="ns8:Engineer" dataDxfId="35">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Engineer" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="27" xr3:uid="{D13CD112-99D7-4A11-8383-F60CFEBAF2BC}" uniqueName="ns8:Genre" name="ns8:Genre" dataDxfId="34">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Genre" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="28" xr3:uid="{13CC3D64-EF4F-4035-A512-E3D898AC83B6}" uniqueName="ns8:Medium" name="ns8:Medium" dataDxfId="33">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Medium" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="29" xr3:uid="{869D406F-22DC-4641-B560-B1A0C69126F9}" uniqueName="ns8:Title" name="ns8:Title" dataDxfId="32">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Title" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="30" xr3:uid="{58D32E4E-80AA-4C4D-A6A2-3AF4367E4DE0}" uniqueName="ns8:Product" name="ns8:Product" dataDxfId="31">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Product" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="31" xr3:uid="{5638AC33-BE08-4273-999D-A24B3707E227}" uniqueName="ns8:SourceForm" name="ns8:SourceForm" dataDxfId="30">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:SourceForm" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="32" xr3:uid="{A594982E-7066-4E88-B5AE-E4151F893EB3}" uniqueName="ns8:Technician" name="ns8:Technician" dataDxfId="29">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Technician" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="33" xr3:uid="{35EBD1ED-244E-47E6-9C98-3ABC122278CF}" uniqueName="ns8:DateTimeOriginal" name="ns8:DateTimeOriginal" dataDxfId="28">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:DateTimeOriginal" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="34" xr3:uid="{CF988176-F21D-4C27-B1EF-31F3407CAC41}" uniqueName="ns8:TimeReference" name="ns8:TimeReference" dataDxfId="27">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:TimeReference" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="35" xr3:uid="{26010328-6E42-4439-BF63-DD7F3B70A7C1}" uniqueName="ns8:BWFVersion" name="ns8:BWFVersion" dataDxfId="26">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:BWFVersion" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="36" xr3:uid="{AB650EDE-2128-4554-A891-3BFEDA57524E}" uniqueName="ns8:BWF_UMID" name="ns8:BWF_UMID" dataDxfId="25">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:BWF_UMID" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="37" xr3:uid="{9B11F7B5-85D0-4831-9969-88524ED96676}" uniqueName="ns8:CodingHistory" name="ns8:CodingHistory" dataDxfId="24">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:CodingHistory" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="38" xr3:uid="{E80F5603-E002-4881-A4D7-61B8634F3167}" uniqueName="ns8:Encoding" name="ns8:Encoding" dataDxfId="23">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Encoding" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="39" xr3:uid="{A70BDCC2-C68F-426D-92CA-B611034913DF}" uniqueName="ns8:NumChannels" name="ns8:NumChannels" dataDxfId="22">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:NumChannels" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="40" xr3:uid="{DDF1A5CE-EDDC-41FB-B95F-E50ED8B3845E}" uniqueName="ns8:SampleRate" name="ns8:SampleRate" dataDxfId="21">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:SampleRate" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="41" xr3:uid="{1D03283B-E5E7-4894-8908-C876C1DAC7D8}" uniqueName="ns8:AvgBytesPerSec" name="ns8:AvgBytesPerSec" dataDxfId="20">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:AvgBytesPerSec" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="42" xr3:uid="{0448BCE5-70E1-4FE2-9C3F-16E5116D8DDA}" uniqueName="ns8:BitsPerSample" name="ns8:BitsPerSample" dataDxfId="19">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:BitsPerSample" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="45" xr3:uid="{3C9BC443-BA6F-4F1F-9E9A-409E4A2335CA}" uniqueName="ns6:Description" name="ns6:Description" dataDxfId="18">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns6:Description" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="46" xr3:uid="{3AE149FC-0C09-4666-84DB-428736C27850}" uniqueName="ns14:ImageSupplierImageID" name="ns14:ImageSupplierImageID" dataDxfId="17">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns14:ImageSupplierImageID" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="47" xr3:uid="{7F33D69E-0907-4583-A51D-4104B2F1DAA7}" uniqueName="ns12:Duration" name="ns12:Duration" dataDxfId="16">
-      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns12:Duration" xmlDataType="string"/>
-    </tableColumn>
+    <tableColumn id="1" xr3:uid="{84AC3680-B818-46E9-BDDF-A3EF93F583DA}" name="ns1:about" dataDxfId="59"/>
+    <tableColumn id="2" xr3:uid="{555E78A8-0450-473A-AA14-7031723405DF}" name="ns13:toolkit" dataDxfId="58"/>
+    <tableColumn id="3" xr3:uid="{14DF793D-F35D-4D72-BD32-C07269818424}" name="ns9:FileName" dataDxfId="57"/>
+    <tableColumn id="4" xr3:uid="{AA5ACBE7-BC21-4294-B3FB-8DE9F2C71F5C}" name="ns9:Directory" dataDxfId="56"/>
+    <tableColumn id="5" xr3:uid="{B3C8E4BF-8614-4B00-995C-5EAD54FE285B}" name="ns9:FileSize" dataDxfId="55"/>
+    <tableColumn id="6" xr3:uid="{AA193ABC-C744-499A-AF6B-41B493117858}" name="ns9:FileModifyDate" dataDxfId="54"/>
+    <tableColumn id="7" xr3:uid="{21A52FD2-4F16-4326-B09D-2B6182F9DDA5}" name="ns9:FileAccessDate" dataDxfId="53"/>
+    <tableColumn id="8" xr3:uid="{301955F4-5866-4A8C-9828-324FFBB14376}" name="ns9:FileCreateDate" dataDxfId="52"/>
+    <tableColumn id="9" xr3:uid="{818119BC-289B-4F12-A8EE-706A13032A32}" name="ns9:FilePermissions" dataDxfId="51"/>
+    <tableColumn id="10" xr3:uid="{0365EBA5-01DF-4B5D-9501-C44963B80C46}" name="ns10:FileType" dataDxfId="50"/>
+    <tableColumn id="11" xr3:uid="{5B2DC416-5DE6-4B35-B152-49D3B675B031}" name="ns10:FileTypeExtension" dataDxfId="49"/>
+    <tableColumn id="12" xr3:uid="{960769D4-B1D1-4385-822B-4E78B88B7B6C}" name="ns10:MIMEType" dataDxfId="48"/>
+    <tableColumn id="13" xr3:uid="{F3F35979-AFE8-4B2C-A442-D424D1F5FA88}" name="ns8:Description" dataDxfId="47"/>
+    <tableColumn id="14" xr3:uid="{392D42CB-EA0E-43F0-8920-ABD08C579264}" name="ns8:Originator" dataDxfId="46"/>
+    <tableColumn id="15" xr3:uid="{5E6F7137-657C-41FF-BB89-3D3A904E3F15}" name="ns8:OriginatorReference" dataDxfId="45"/>
+    <tableColumn id="16" xr3:uid="{C252949A-FDE9-47AE-A261-8F678F6EF023}" name="ns8:Artist" dataDxfId="44"/>
+    <tableColumn id="17" xr3:uid="{99D1567D-BEAD-4DE4-81B1-2763ACB5640E}" name="ns8:Commissioned" dataDxfId="43"/>
+    <tableColumn id="18" xr3:uid="{20457787-E9B1-4B87-B26A-D08F8F5F288E}" name="ns8:DateCreated" dataDxfId="42"/>
+    <tableColumn id="19" xr3:uid="{FF856206-A27C-4184-947E-F8A3409FC987}" name="ns8:Keywords" dataDxfId="41"/>
+    <tableColumn id="20" xr3:uid="{55C4F58F-AF8D-4320-90B3-F6A10D930675}" name="ns8:Subject" dataDxfId="40"/>
+    <tableColumn id="21" xr3:uid="{DB22375E-DB09-49BC-AF9F-00B6D6DE8313}" name="ns8:Software" dataDxfId="39"/>
+    <tableColumn id="22" xr3:uid="{10656292-9695-4CA9-AB4D-CC76886BE4BC}" name="ns8:Source" dataDxfId="38"/>
+    <tableColumn id="23" xr3:uid="{C8C6413A-1FB7-4A8F-9748-EBBBFA52F888}" name="ns8:ArchivalLocation" dataDxfId="37"/>
+    <tableColumn id="24" xr3:uid="{FD5867F6-7FEB-46AD-910E-F5AF840FE10C}" name="ns8:Comment" dataDxfId="36"/>
+    <tableColumn id="25" xr3:uid="{1BFA4B4E-CFC1-4C43-9DF9-737B02498676}" name="ns8:Copyright" dataDxfId="35"/>
+    <tableColumn id="26" xr3:uid="{54BF07E3-6137-41E9-B763-9B5FB5CEE0EC}" name="ns8:Engineer" dataDxfId="34"/>
+    <tableColumn id="27" xr3:uid="{C901C0BF-CF6D-413C-AC28-C740E2C26255}" name="ns8:Genre" dataDxfId="33"/>
+    <tableColumn id="28" xr3:uid="{1A82BB1D-A422-4E4A-A31F-323E1593585E}" name="ns8:Medium" dataDxfId="32"/>
+    <tableColumn id="29" xr3:uid="{80F3CAE0-23C7-46D0-BE10-E49EC6290026}" name="ns8:Title" dataDxfId="31"/>
+    <tableColumn id="30" xr3:uid="{8899EB6B-EAD4-4F0B-9FB8-C31E12E2F0F2}" name="ns8:Product" dataDxfId="30"/>
+    <tableColumn id="31" xr3:uid="{52D4A082-E79A-424A-A9BF-A1028F563355}" name="ns8:SourceForm" dataDxfId="29"/>
+    <tableColumn id="32" xr3:uid="{A712999D-8892-4926-A8A7-108BD7B637A3}" name="ns8:Technician" dataDxfId="28"/>
+    <tableColumn id="33" xr3:uid="{E93EC693-3550-44C3-AC4C-5E39137FAE12}" name="ns8:DateTimeOriginal" dataDxfId="27"/>
+    <tableColumn id="34" xr3:uid="{4752B2BF-2AEE-4754-9BB2-F6182E1F892F}" name="ns8:TimeReference" dataDxfId="26"/>
+    <tableColumn id="35" xr3:uid="{3923428A-1650-440B-BD97-F44404EECA13}" name="ns8:BWFVersion" dataDxfId="25"/>
+    <tableColumn id="36" xr3:uid="{94473350-F58B-4F01-BD34-8BADCE99E8DC}" name="ns8:BWF_UMID" dataDxfId="24"/>
+    <tableColumn id="37" xr3:uid="{E3BF5021-62DB-4B48-BE9F-C6949A8E67A1}" name="ns8:CodingHistory" dataDxfId="23"/>
+    <tableColumn id="38" xr3:uid="{3B96C7B0-2D4E-46E9-8A94-6E264FA59A38}" name="ns8:Encoding" dataDxfId="22"/>
+    <tableColumn id="39" xr3:uid="{40EE75C2-3405-4DC0-A175-00E1EC4476B5}" name="ns8:NumChannels" dataDxfId="21"/>
+    <tableColumn id="40" xr3:uid="{462CA8E8-1DA9-424C-A843-67F58550147D}" name="ns8:SampleRate" dataDxfId="20"/>
+    <tableColumn id="41" xr3:uid="{452367F2-AF7F-4F8D-8976-D4A6D4688BF2}" name="ns8:AvgBytesPerSec" dataDxfId="19"/>
+    <tableColumn id="42" xr3:uid="{56C06A66-E2DE-4F21-8CA5-50873B0D9822}" name="ns8:BitsPerSample" dataDxfId="18"/>
+    <tableColumn id="45" xr3:uid="{64FB92C2-AC51-44EE-BE84-FAA0E897A3DE}" name="ns6:Description" dataDxfId="17"/>
+    <tableColumn id="46" xr3:uid="{E216F627-30BE-41B7-84FA-CD0F528A9491}" name="ns14:ImageSupplierImageID" dataDxfId="16"/>
+    <tableColumn id="47" xr3:uid="{983F0130-6BC7-46EA-8133-B6341865E6FD}" name="ns12:Duration" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{58EE3EDB-2EE9-41D7-B2DD-D62B12E6E8DE}" name="Table111" displayName="Table111" ref="A1:M2" tableType="xml" insertRow="1" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" connectionId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0445CE99-DC86-4685-A3DF-1B4B786F25F0}" name="Table1113" displayName="Table1113" ref="A1:M2" insertRow="1" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:M2" xr:uid="{7F6E844D-01BA-4C52-9E71-607021A40716}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{AE7A3A3E-FEF7-4E50-AE78-63635D11553D}" uniqueName="instantiationID" name="instantiationID" dataDxfId="13">
-      <xmlColumnPr mapId="4" xpath="/instantiationIDs/instantiationID" xmlDataType="double"/>
-    </tableColumn>
-    <tableColumn id="2" xr3:uid="{F579EB87-213F-47BF-8889-A4CB9D1EEA4F}" uniqueName="format" name="format" dataDxfId="12">
-      <xmlColumnPr mapId="4" xpath="/instantiationIDs/instantiationID/@format" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="18" xr3:uid="{4F24F387-B82B-48C7-97F9-66E03F47B260}" uniqueName="18" name="location" dataDxfId="10"/>
-    <tableColumn id="19" xr3:uid="{7582DD9D-46D7-45DB-B2AE-6B718660D8E5}" uniqueName="19" name="title" dataDxfId="9"/>
-    <tableColumn id="20" xr3:uid="{14538894-9334-45F7-89F6-9CD39007C16E}" uniqueName="20" name="earliestDate" dataDxfId="8"/>
-    <tableColumn id="21" xr3:uid="{B26B4A75-0CDD-42D5-BE43-49468463C738}" uniqueName="21" name="url" dataDxfId="7"/>
-    <tableColumn id="22" xr3:uid="{8FAEACC3-FCB4-4E4F-8E55-FAE6B785AF16}" uniqueName="22" name="series" dataDxfId="6"/>
-    <tableColumn id="23" xr3:uid="{DC5B3CB5-BB31-49EC-8EA0-FC6ABF61F528}" uniqueName="23" name="collection" dataDxfId="5"/>
-    <tableColumn id="24" xr3:uid="{50A9081E-0BBE-4759-95BB-364D5F1577C8}" uniqueName="24" name="allDates" dataDxfId="4"/>
-    <tableColumn id="25" xr3:uid="{184A2C95-3314-4AF2-8D13-CBDE92B21B96}" uniqueName="25" name="otherIDs" dataDxfId="3"/>
-    <tableColumn id="28" xr3:uid="{10457911-A7B8-4C0B-A90D-14E88BFE20C2}" uniqueName="28" name="photoLocator" dataDxfId="0"/>
-    <tableColumn id="26" xr3:uid="{AC3A77EA-8968-4F1B-BAD1-6E9E0EC15279}" uniqueName="26" name="futureShelf" dataDxfId="2"/>
-    <tableColumn id="27" xr3:uid="{F0A027E8-A875-4852-91FC-C696F0860B26}" uniqueName="27" name="futureBox" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{759CE8EF-4705-4CA7-9E98-7C7AF1E8A3A1}" name="instantiationID" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{24F11AEC-A8D7-4E89-9557-657383C6E023}" name="format" dataDxfId="11"/>
+    <tableColumn id="18" xr3:uid="{B30E2AAF-1D86-4E21-9CE7-AAA86835D945}" name="location" dataDxfId="10"/>
+    <tableColumn id="19" xr3:uid="{57D867EF-5B64-425F-ACEF-F65F5678C159}" name="title" dataDxfId="9"/>
+    <tableColumn id="20" xr3:uid="{DFBB673C-8187-4B74-8B6B-770833313A6B}" name="earliestDate" dataDxfId="8"/>
+    <tableColumn id="21" xr3:uid="{8B33B58F-F358-491A-A023-D6C5CDF45AD1}" name="url" dataDxfId="7"/>
+    <tableColumn id="22" xr3:uid="{8108A980-58F1-4202-9CE2-D7253005D1F5}" name="series" dataDxfId="6"/>
+    <tableColumn id="23" xr3:uid="{25E297E4-772F-4135-9EC3-71CEC854D24D}" name="collection" dataDxfId="5"/>
+    <tableColumn id="24" xr3:uid="{E8FA4467-FFDA-43A0-AF23-D4D6736D3A99}" name="allDates" dataDxfId="4"/>
+    <tableColumn id="25" xr3:uid="{BF9E90CA-D525-4A3B-AAB5-A4225232C7A3}" name="otherIDs" dataDxfId="3"/>
+    <tableColumn id="28" xr3:uid="{FAA919DC-F11B-46E5-A251-AAFF973B5F4B}" name="photoLocator" dataDxfId="2"/>
+    <tableColumn id="26" xr3:uid="{F20260DB-1D2D-44DB-AF45-A0E4BF5A4178}" name="futureShelf" dataDxfId="1"/>
+    <tableColumn id="27" xr3:uid="{B530A3D3-B604-4F2E-A4C9-B0695BC04D07}" name="futureBox" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{152F4DBB-82EC-4174-B546-903AE163E78E}" name="Table9" displayName="Table9" ref="A1:AS2" tableType="xml" totalsRowShown="0" headerRowDxfId="109" dataDxfId="108" connectionId="2">
+  <autoFilter ref="A1:AS2" xr:uid="{DBA4640A-ED60-420F-906F-CF4D7DD1EE4D}"/>
+  <tableColumns count="45">
+    <tableColumn id="1" xr3:uid="{A580D164-B803-461C-9F4F-A5883098A8DC}" uniqueName="ns1:about" name="ns1:about" dataDxfId="107">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/@ns1:about" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{05AC7C08-38B5-4261-A443-BEA6080FEDDA}" uniqueName="ns13:toolkit" name="ns13:toolkit" dataDxfId="106">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/@ns13:toolkit" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{A5EA5A7D-DF33-4A97-82BB-0A7F0753F4DF}" uniqueName="ns9:FileName" name="ns9:FileName" dataDxfId="105">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns9:FileName" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{EA4A8834-6D73-4C7F-B6AF-389D2D43DD68}" uniqueName="ns9:Directory" name="ns9:Directory" dataDxfId="104">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns9:Directory" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{67463FDA-5FD6-4B14-9F81-FE55D0178052}" uniqueName="ns9:FileSize" name="ns9:FileSize" dataDxfId="103">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns9:FileSize" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{0C3060F6-F8A0-4D82-AAC7-1BDA75963948}" uniqueName="ns9:FileModifyDate" name="ns9:FileModifyDate" dataDxfId="102">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns9:FileModifyDate" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{D8247E8D-6713-454E-918C-65CF07DFD18E}" uniqueName="ns9:FileAccessDate" name="ns9:FileAccessDate" dataDxfId="101">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns9:FileAccessDate" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{314C7B67-1EA1-4F9B-9BA8-65CEF7058C26}" uniqueName="ns9:FileCreateDate" name="ns9:FileCreateDate" dataDxfId="100">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns9:FileCreateDate" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{FE9CC9E5-2BD9-46CA-8DDF-367714039F6E}" uniqueName="ns9:FilePermissions" name="ns9:FilePermissions" dataDxfId="99">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns9:FilePermissions" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{A745FD77-9ADB-44D6-8904-007E5A609840}" uniqueName="ns10:FileType" name="ns10:FileType" dataDxfId="98">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns10:FileType" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{BC259896-1D6F-4AE7-A726-B8834A69BBC2}" uniqueName="ns10:FileTypeExtension" name="ns10:FileTypeExtension" dataDxfId="97">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns10:FileTypeExtension" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="12" xr3:uid="{BBE38AEA-ECEB-4766-8AB0-933A72D382A8}" uniqueName="ns10:MIMEType" name="ns10:MIMEType" dataDxfId="96">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns10:MIMEType" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="13" xr3:uid="{39257707-B95F-45C9-AC76-F1FCA3BBF450}" uniqueName="ns8:Description" name="ns8:Description" dataDxfId="95">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Description" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="14" xr3:uid="{9CA1E0C7-3686-4C63-B1BF-25AB0784699E}" uniqueName="ns8:Originator" name="ns8:Originator" dataDxfId="94">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Originator" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="15" xr3:uid="{7087961F-8AA4-489C-9EF6-98485712B62A}" uniqueName="ns8:OriginatorReference" name="ns8:OriginatorReference" dataDxfId="93">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:OriginatorReference" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="16" xr3:uid="{C73D8355-013C-400C-A0A9-EFE01E3D050B}" uniqueName="ns8:Artist" name="ns8:Artist" dataDxfId="92">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Artist" xmlDataType="anyURI"/>
+    </tableColumn>
+    <tableColumn id="17" xr3:uid="{D13DCDF0-0CC2-4BCB-AFDF-2CF798AFE524}" uniqueName="ns8:Commissioned" name="ns8:Commissioned" dataDxfId="91">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Commissioned" xmlDataType="anyURI"/>
+    </tableColumn>
+    <tableColumn id="18" xr3:uid="{02063AF9-BF3F-4FF1-8D86-A9A5A1240A73}" uniqueName="ns8:DateCreated" name="ns8:DateCreated" dataDxfId="90">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:DateCreated" xmlDataType="date"/>
+    </tableColumn>
+    <tableColumn id="19" xr3:uid="{BB997E4E-ED1D-4A6D-8A24-A863681A2E20}" uniqueName="ns8:Keywords" name="ns8:Keywords" dataDxfId="89">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Keywords" xmlDataType="anyURI"/>
+    </tableColumn>
+    <tableColumn id="20" xr3:uid="{48BC8FF1-7BFE-41C9-9C48-F8DC04E14800}" uniqueName="ns8:Subject" name="ns8:Subject" dataDxfId="88">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Subject" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="21" xr3:uid="{5120FA96-3590-4F48-8545-6E4CC51A5B49}" uniqueName="ns8:Software" name="ns8:Software" dataDxfId="87">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Software" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="22" xr3:uid="{58933FB6-0CDD-4BB3-837C-451A48F41091}" uniqueName="ns8:Source" name="ns8:Source" dataDxfId="86">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Source" xmlDataType="anyURI"/>
+    </tableColumn>
+    <tableColumn id="23" xr3:uid="{6DB07D3F-F109-424F-9423-952C9C1F0F68}" uniqueName="ns8:ArchivalLocation" name="ns8:ArchivalLocation" dataDxfId="85">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:ArchivalLocation" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="24" xr3:uid="{32999CD4-C6BA-4922-B7AA-328EC1D95C5C}" uniqueName="ns8:Comment" name="ns8:Comment" dataDxfId="84">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Comment" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="25" xr3:uid="{88B06FCA-C7DB-4AFE-8C8A-9156B064162B}" uniqueName="ns8:Copyright" name="ns8:Copyright" dataDxfId="83">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Copyright" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="26" xr3:uid="{78765629-CBE4-402A-9D4E-E90C72C8BF39}" uniqueName="ns8:Engineer" name="ns8:Engineer" dataDxfId="82">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Engineer" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="27" xr3:uid="{D13CD112-99D7-4A11-8383-F60CFEBAF2BC}" uniqueName="ns8:Genre" name="ns8:Genre" dataDxfId="81">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Genre" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="28" xr3:uid="{13CC3D64-EF4F-4035-A512-E3D898AC83B6}" uniqueName="ns8:Medium" name="ns8:Medium" dataDxfId="80">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Medium" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="29" xr3:uid="{869D406F-22DC-4641-B560-B1A0C69126F9}" uniqueName="ns8:Title" name="ns8:Title" dataDxfId="79">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Title" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="30" xr3:uid="{58D32E4E-80AA-4C4D-A6A2-3AF4367E4DE0}" uniqueName="ns8:Product" name="ns8:Product" dataDxfId="78">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Product" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="31" xr3:uid="{5638AC33-BE08-4273-999D-A24B3707E227}" uniqueName="ns8:SourceForm" name="ns8:SourceForm" dataDxfId="77">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:SourceForm" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="32" xr3:uid="{A594982E-7066-4E88-B5AE-E4151F893EB3}" uniqueName="ns8:Technician" name="ns8:Technician" dataDxfId="76">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Technician" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="33" xr3:uid="{35EBD1ED-244E-47E6-9C98-3ABC122278CF}" uniqueName="ns8:DateTimeOriginal" name="ns8:DateTimeOriginal" dataDxfId="75">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:DateTimeOriginal" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="34" xr3:uid="{CF988176-F21D-4C27-B1EF-31F3407CAC41}" uniqueName="ns8:TimeReference" name="ns8:TimeReference" dataDxfId="74">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:TimeReference" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="35" xr3:uid="{26010328-6E42-4439-BF63-DD7F3B70A7C1}" uniqueName="ns8:BWFVersion" name="ns8:BWFVersion" dataDxfId="73">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:BWFVersion" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="36" xr3:uid="{AB650EDE-2128-4554-A891-3BFEDA57524E}" uniqueName="ns8:BWF_UMID" name="ns8:BWF_UMID" dataDxfId="72">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:BWF_UMID" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="37" xr3:uid="{9B11F7B5-85D0-4831-9969-88524ED96676}" uniqueName="ns8:CodingHistory" name="ns8:CodingHistory" dataDxfId="71">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:CodingHistory" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="38" xr3:uid="{E80F5603-E002-4881-A4D7-61B8634F3167}" uniqueName="ns8:Encoding" name="ns8:Encoding" dataDxfId="70">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:Encoding" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="39" xr3:uid="{A70BDCC2-C68F-426D-92CA-B611034913DF}" uniqueName="ns8:NumChannels" name="ns8:NumChannels" dataDxfId="69">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:NumChannels" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="40" xr3:uid="{DDF1A5CE-EDDC-41FB-B95F-E50ED8B3845E}" uniqueName="ns8:SampleRate" name="ns8:SampleRate" dataDxfId="68">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:SampleRate" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="41" xr3:uid="{1D03283B-E5E7-4894-8908-C876C1DAC7D8}" uniqueName="ns8:AvgBytesPerSec" name="ns8:AvgBytesPerSec" dataDxfId="67">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:AvgBytesPerSec" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="42" xr3:uid="{0448BCE5-70E1-4FE2-9C3F-16E5116D8DDA}" uniqueName="ns8:BitsPerSample" name="ns8:BitsPerSample" dataDxfId="66">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns8:BitsPerSample" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="45" xr3:uid="{3C9BC443-BA6F-4F1F-9E9A-409E4A2335CA}" uniqueName="ns6:Description" name="ns6:Description" dataDxfId="65">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns6:Description" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="46" xr3:uid="{3AE149FC-0C09-4666-84DB-428736C27850}" uniqueName="ns14:ImageSupplierImageID" name="ns14:ImageSupplierImageID" dataDxfId="64">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns14:ImageSupplierImageID" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="47" xr3:uid="{7F33D69E-0907-4583-A51D-4104B2F1DAA7}" uniqueName="ns12:Duration" name="ns12:Duration" dataDxfId="63">
+      <xmlColumnPr mapId="3" xpath="/ns1:RDF/ns1:Description/ns12:Duration" xmlDataType="string"/>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A2E66EFD-4DDC-4BD4-B8C5-AED44F3C3B04}" name="Table1" displayName="Table1" ref="A1:B2" insertRow="1" totalsRowShown="0">
   <autoFilter ref="A1:B2" xr:uid="{C33A8AF7-B6D4-4C4A-B138-B8308E1B085D}"/>
   <tableColumns count="2">
@@ -1133,14 +1348,14 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{5D1E2B19-8C39-4E3A-A0FA-50DF2B2D631A}" name="format" displayName="format" ref="A1:A31" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:A31" xr:uid="{221B5900-A88D-4E6B-9C5D-C153444136E4}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A31">
     <sortCondition ref="A1:A31"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{C82B992E-A0B3-43B5-A398-30A2E780747E}" uniqueName="1" name="Element:Text" queryTableFieldId="1" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{C82B992E-A0B3-43B5-A398-30A2E780747E}" uniqueName="1" name="Element:Text" queryTableFieldId="1" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1442,76 +1657,76 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45CF6150-5B4C-4370-88BD-95E6691BC622}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF625C72-F81B-4FCA-9FE6-CA2194CED492}">
   <dimension ref="A1:BF2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="BD2" sqref="BD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.54296875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.7265625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="21" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="25.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="25.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="21.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="14.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="17.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="22.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="20.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="21.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="17.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="19.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="14.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="19.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="17.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="21.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="17.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="59" max="16384" width="11.85546875" style="1"/>
+    <col min="56" max="56" width="17.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="28.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="15.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="59" max="16384" width="11.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>86</v>
       </c>
@@ -1687,7 +1902,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1711,7 +1926,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F561371C-BF36-486A-8A07-D9C502CAE1E4}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0129390A-E75D-4C2B-A001-D2CBB7862328}">
           <x14:formula1>
             <xm:f>vocabularies!$A$2:$A$31</xm:f>
           </x14:formula1>
@@ -1724,18 +1939,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F05020F-896E-4447-A3D5-32141EA427B8}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7749DA7D-0BA9-4337-B89F-3A700811011F}">
   <dimension ref="A1:AQ3"/>
   <sheetViews>
@@ -1745,12 +1948,12 @@
       <selection pane="bottomLeft" activeCell="AJ2" sqref="AJ2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="24.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="24.85546875" style="2"/>
+    <col min="1" max="16384" width="24.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1881,7 +2084,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:43" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>45</v>
       </c>
@@ -2018,15 +2221,276 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F05020F-896E-4447-A3D5-32141EA427B8}">
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I1" t="s">
+        <v>132</v>
+      </c>
+      <c r="J1" t="s">
+        <v>134</v>
+      </c>
+      <c r="K1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98B7391A-B7EA-44A8-BD19-0B72196963EF}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45CF6150-5B4C-4370-88BD-95E6691BC622}">
+  <dimension ref="A1:AS2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M1" sqref="A1:M1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="11.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="22.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="20.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="17.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="19.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="19.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="21.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="17.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="28.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="15.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="16384" width="11.81640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -2038,13 +2502,13 @@
       <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.26953125" customWidth="1"/>
+    <col min="2" max="2" width="9.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>86</v>
       </c>
@@ -2052,7 +2516,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B2" s="1"/>
     </row>
   </sheetData>
@@ -2082,12 +2546,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="144.140625" customWidth="1"/>
+    <col min="1" max="1" width="144.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="270" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>119</v>
       </c>
@@ -2105,162 +2569,162 @@
       <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>88</v>
       </c>

</xml_diff>